<commit_message>
Rerun data analysis pipeline
</commit_message>
<xml_diff>
--- a/scripts/ratings.xlsx
+++ b/scripts/ratings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,24 +465,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>0zPmxcWjnYVNWRxC0FQ5</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0qqwGIKuUk9YUJeWTuXE</t>
+          <t>25Hk9N0KYy91RxCins7P</t>
         </is>
       </c>
     </row>
@@ -491,24 +491,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5c4de518-ce97-4abf-afb7-262a7aceaf38</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>5J9RGqRBu4bbBpQTXt2F</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1vcFDWJrTKct97YYbNWS</t>
+          <t>2Gz1GdZcXYHalo0x8eRu</t>
         </is>
       </c>
     </row>
@@ -521,12 +521,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>1ECYj3ZwNcAGd0YvCx3V</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -534,7 +534,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2nRJa9SKRgUZBHy9Ti9w</t>
+          <t>3EsaNRJ5y9cx6LOfwXev</t>
         </is>
       </c>
     </row>
@@ -547,20 +547,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>5mZGDS5EilurdRWbyGlD</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2xm3gM2JH2xFvmdwcuTw</t>
+          <t>48szEt3tdRLqmi2FfIqN</t>
         </is>
       </c>
     </row>
@@ -569,24 +569,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>4mugp0USuNw8iuDR2GWw</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3d5uxrbpISUZwqUgAqgZ</t>
+          <t>7HwhmofD6lkpRE6o9apO</t>
         </is>
       </c>
     </row>
@@ -595,24 +595,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>80UVZls1IQNjKgrKfy5v</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5kJg8j3XbRfeWCtaBFvM</t>
+          <t>7ICUOAfMb8EqApkgcody</t>
         </is>
       </c>
     </row>
@@ -621,24 +621,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>5JzFVmuTbG1nMFIrap6x</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6gCLeiiySvJqJaJJqnjA</t>
+          <t>89YHgSA4NdL1Fze1x2dX</t>
         </is>
       </c>
     </row>
@@ -651,20 +651,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>41MDpaRtPVIASNhgdgsT</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BFtNBqBURJxgSdzCW2mV</t>
+          <t>B85crgfCgXHQG3ehm5Hn</t>
         </is>
       </c>
     </row>
@@ -677,20 +677,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>4h3sZUmpzXkiw2vcZEin</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>BYpqFnXoG798x89yPjrB</t>
+          <t>CeR6xJd55m9GK5HhNp7i</t>
         </is>
       </c>
     </row>
@@ -703,12 +703,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>995821fa-fef4-4f69-8a52-9b06d59c36d8</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>1l4HXH7ntrCxNIIbHror</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -716,7 +716,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>D02TI66k0KkLlSwyC1vI</t>
+          <t>CyjVoZ81RZdnxuFnolWI</t>
         </is>
       </c>
     </row>
@@ -725,24 +725,24 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>3O8o4gAOjJ2CtgNxSWis</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>FRzKcvM2qDxjdxZo8eF0</t>
+          <t>DuQ7lMIddWxh9yaag4qR</t>
         </is>
       </c>
     </row>
@@ -751,24 +751,24 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>2VkrluqdREPySkjAYqEi</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Gn38dwXPJMkc6atb85Ts</t>
+          <t>FRE6sRulYE6IWO5CIpxY</t>
         </is>
       </c>
     </row>
@@ -777,24 +777,24 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>4sAfxBA65oCTMjZBKkck</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>HW547B3H7RPTUk76u6ZH</t>
+          <t>IVaSb7vZn6wlEuz4Qx4N</t>
         </is>
       </c>
     </row>
@@ -807,20 +807,20 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>5Wfdge4zYyfRmyYV1Pv2</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>I2LzRMfhuE2bk5Ydlg9R</t>
+          <t>JLdVShZiovzwmN3nrwtM</t>
         </is>
       </c>
     </row>
@@ -833,12 +833,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>84af58d9-1067-403c-8724-8272d3901ce1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>6qOEqprzqwIaVimYC6CE</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -846,7 +846,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>JgJOZ80CInxIdRsdsUe3</t>
+          <t>KClPuDKLHh0lN9wVBDJX</t>
         </is>
       </c>
     </row>
@@ -859,20 +859,20 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>4b5lryRnNp83iTqLcbjy</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>KkxE0iqQ8yIsrxqi21OS</t>
+          <t>LqW28xV2NI0kJYBlZ8tp</t>
         </is>
       </c>
     </row>
@@ -885,20 +885,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>6ZOSY7q1l5yylubvkSJL</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>KrJUCSEM10FXqEkLqikq</t>
+          <t>LtFFtBekOwtpuNLXvPA5</t>
         </is>
       </c>
     </row>
@@ -911,12 +911,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>08bsHQhNX79lPv5Xe2Tb</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -924,7 +924,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>LfZ6aMp1P25DjHztGKjV</t>
+          <t>Ma16d3X1RcogQkjIQBoE</t>
         </is>
       </c>
     </row>
@@ -937,12 +937,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>30KZjXBTWPzyYTDoMNGY</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -950,7 +950,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Mlv6RNi4MmvHRR9oLvJk</t>
+          <t>Rft99WPdFouVqgKpMTwu</t>
         </is>
       </c>
     </row>
@@ -959,24 +959,24 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>1ENYbKRV8yNpaHGfWSgs</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>NpCQGKvv62XdyK4K4N3a</t>
+          <t>UzEpX0FlxcZCvGR8Mf3O</t>
         </is>
       </c>
     </row>
@@ -989,20 +989,20 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>1vV79xXL4ZS0yJnZqiOW</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>PF8W1w4VOWZyUchSui4f</t>
+          <t>aEkMwjs5SZMxwe4Aa6Uq</t>
         </is>
       </c>
     </row>
@@ -1011,24 +1011,24 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>9Gh6ruf8aSDdISAf85ni</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>PdJqAstWi9kVehWE3AxT</t>
+          <t>iUzHd8mXywBwY4jjmrRr</t>
         </is>
       </c>
     </row>
@@ -1037,24 +1037,24 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>3xvQDJNzy0A1EcxRHX3c</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PhbCHezTkzTl3gkwCF5U</t>
+          <t>mpeQwVdiNJPoXnCqEDXg</t>
         </is>
       </c>
     </row>
@@ -1067,20 +1067,20 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
+          <t>6a3bde48-d694-46e1-9b93-c469d3f067dc</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>3oViwh66ISTJUEsyQpSN</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>QQSgn4ELWsiTe99HL6WN</t>
+          <t>oRu2evXf9VPfwnmYKqar</t>
         </is>
       </c>
     </row>
@@ -1093,20 +1093,20 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
+          <t>995821fa-fef4-4f69-8a52-9b06d59c36d8</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>10ogClgsmLKNyvRwQsTW</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>S7Xw1LKz3e5GBURl09xG</t>
+          <t>sOMDUUrjolTZFo6JwMHp</t>
         </is>
       </c>
     </row>
@@ -1115,16 +1115,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
+          <t>4n0RqjnuVCVc8lFDoguk</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Sm6KTwNfMnU3DAcXaQo1</t>
+          <t>vsNIUxTSYOSI2ysDrA7R</t>
         </is>
       </c>
     </row>
@@ -1141,24 +1141,24 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>d5ed6f59-5f4c-40ef-a9aa-0d8f4c930b48</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
+          <t>3CrFCIb4ejCumrz2ElX5</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Wm0PNk31XidAdvgB9iUo</t>
+          <t>wWck85HKAfHaihZA1yei</t>
         </is>
       </c>
     </row>
@@ -1171,12 +1171,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
+          <t>237834c1-fed1-479e-8882-b3adcc0f4188</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
+          <t>956ZyPUN2no8bwtH1HvW</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>YJRUth4VKmEJu7ZGHZUg</t>
+          <t>whx9OOC0pZXayrEVmHwn</t>
         </is>
       </c>
     </row>
@@ -1193,596 +1193,24 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
+          <t>98f7b383-764c-4a7d-b44a-6aec8aeb8eda</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
+          <t>2LoqnwOxieF56jPhYYZo</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>YShT4GJbXiVYmuGPYfv4</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>5</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>3</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>YfDRb7OoqCOITLgrx6o6</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>5</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>4</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>ZbH7tjihyIQt9mSt4tJ7</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>5</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>4</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>auIVdqOLOFrTiIklzLOH</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>5</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>3</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>bqL1bP6yvqg9BdTRSfCK</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>5</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>4</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>e4KDxqXTn1jw5wXNk4Jg</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>3</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>b129d86a-4077-4b49-8494-4942b76bfbb1</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>5</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>eurKXa2qR74n9sOpw4X0</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>5</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>4</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>f5VH7LoeUZ1vFn3KwwMJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>5</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>3</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>fWkHIypCw0ZBbMZqG0MJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>5</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>5</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>g0wWHwMNU1K3lxEx5LDH</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="n">
-        <v>5</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>3</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>g9Asnc908r05woHBCOlm</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="n">
-        <v>3</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>4</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>hJMVI1CTbDSS4108H6Qp</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>5</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>3</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>hsCX7T7tqPKrlJp6WCcH</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="n">
-        <v>4</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>4825af3c-d463-4c5c-ac54-781f3890c126</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>4</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>iAQ9g8XGZ9ik4QY9CUdZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="n">
-        <v>4</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>3e5c9d3b-36d6-44c1-8a48-2218bee521c6</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>BGOjoywll3sSUYo2pBwY</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>5</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>kN9iY9GnTUzAMo5RIwjZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>5</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>5</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>mGHQIp9Gv18rSmj7J1Uj</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="n">
-        <v>5</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>4</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>nUQnCCzBMpXrnwVw7i60</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>5dwojHXzFd2RzJ2ZPNtD</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>4</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>r7wSm69NXcryXpd5eZIQ</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="n">
-        <v>4</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>4825af3c-d463-4c5c-ac54-781f3890c126</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>4</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>tvllY9jEMZ4FEdMYjpzt</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="n">
-        <v>5</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>40096913-7fd3-40ca-a486-8f38c30ef030</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>3</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>uUoOq0dxcJb84PIHAD3x</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="n">
-        <v>3</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>d5ed6f59-5f4c-40ef-a9aa-0d8f4c930b48</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>5</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>xRRIvdDlH0BG453SGVSz</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="n">
-        <v>5</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>9e521ca6-c80c-4128-91ad-a72a35a6988c</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>PqpflZDmB5tBiM15v9MQ</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>4</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>xWfMHNkxPkMZVWdjTcHb</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="n">
-        <v>4</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>ae868375-47d2-4b8a-995b-66e8e33ebf0a</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>OyhrkDZsWy64SkqfZAY5</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>2</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>yHra9FHoHYK939FWtJEc</t>
+          <t>zQYxBxujLtLtJGvHjYja</t>
         </is>
       </c>
     </row>

</xml_diff>